<commit_message>
finalize the customer_segmentation part
</commit_message>
<xml_diff>
--- a/07_Project_Capstone_Arvato-Bertelsmann/data/description/DIAS Attributes - Values 2017.xlsx
+++ b/07_Project_Capstone_Arvato-Bertelsmann/data/description/DIAS Attributes - Values 2017.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trw1-my.sharepoint.com/personal/robin_wesselmann_zf_com/Documents/Desktop/Udacity_DataScientist_Class/07_Project_Capstone_Arvato-Bertelsmann/data/description/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z635177\OneDrive - ZF Friedrichshafen AG\Desktop\Udacity_DataScientist_Class\07_Project_Capstone_Arvato-Bertelsmann\data\description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_A1335B4F17C50433E16D7E62698543FD2E9B5F63" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17A1A3BF-7B1F-46E7-BF71-DA6BDE3735BC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0159C989-BA61-4438-B377-DFFD8E36A281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="original_data" sheetId="1" r:id="rId1"/>
@@ -4429,13 +4429,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A638" workbookViewId="0">
-      <selection activeCell="C657" sqref="C657:C659"/>
+    <sheetView tabSelected="1" topLeftCell="A660" workbookViewId="0">
+      <selection activeCell="B693" sqref="B693"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="53.42578125" customWidth="1"/>
     <col min="3" max="3" width="5.28515625" style="1" customWidth="1"/>
     <col min="4" max="5" width="76.140625" customWidth="1"/>
@@ -46712,12 +46712,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46770,15 +46767,24 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3EA3FA-F7A9-4EB1-BDA9-02346FC3DB01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBE20A7-1A06-4982-8E6C-B0692E74AD85}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -46799,15 +46805,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBE20A7-1A06-4982-8E6C-B0692E74AD85}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3EA3FA-F7A9-4EB1-BDA9-02346FC3DB01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>